<commit_message>
All canvas done and fixed.
</commit_message>
<xml_diff>
--- a/Demomax.xlsx
+++ b/Demomax.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2455" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2581" uniqueCount="119">
   <si>
     <t>Surname</t>
   </si>
@@ -367,6 +367,15 @@
   </si>
   <si>
     <t>Bobla</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>13.07.2013</t>
+  </si>
+  <si>
+    <t>15.08.2012</t>
   </si>
 </sst>
 </file>
@@ -774,11 +783,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S175"/>
+  <dimension ref="A1:S184"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B184" sqref="A184:XFD184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11128,6 +11137,537 @@
       </c>
       <c r="S175" s="1" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="176" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A176" s="1">
+        <v>8456987</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G176" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H176" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I176" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J176" s="12">
+        <v>41432</v>
+      </c>
+      <c r="K176" s="10">
+        <v>41434</v>
+      </c>
+      <c r="L176" s="1">
+        <v>3</v>
+      </c>
+      <c r="M176" s="1">
+        <v>150</v>
+      </c>
+      <c r="N176" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O176" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P176" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q176" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R176" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="S176" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="177" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A177" s="1">
+        <v>8456987</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G177" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H177" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I177" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J177" s="12">
+        <v>41432</v>
+      </c>
+      <c r="K177" s="10">
+        <v>41434</v>
+      </c>
+      <c r="L177" s="1">
+        <v>3</v>
+      </c>
+      <c r="M177" s="1">
+        <v>150</v>
+      </c>
+      <c r="N177" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O177" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P177" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q177" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R177" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="S177" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="178" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A178" s="1">
+        <v>8456987</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G178" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H178" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I178" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J178" s="12">
+        <v>41432</v>
+      </c>
+      <c r="K178" s="10">
+        <v>41434</v>
+      </c>
+      <c r="L178" s="1">
+        <v>3</v>
+      </c>
+      <c r="M178" s="1">
+        <v>150</v>
+      </c>
+      <c r="N178" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O178" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P178" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q178" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R178" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="S178" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="179" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A179" s="1">
+        <v>8456987</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F179" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G179" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H179" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I179" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J179" s="12">
+        <v>41432</v>
+      </c>
+      <c r="K179" s="10">
+        <v>41434</v>
+      </c>
+      <c r="L179" s="1">
+        <v>3</v>
+      </c>
+      <c r="M179" s="1">
+        <v>150</v>
+      </c>
+      <c r="N179" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O179" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P179" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q179" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R179" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="S179" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="180" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A180" s="1">
+        <v>8456987</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G180" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H180" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I180" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J180" s="12">
+        <v>41432</v>
+      </c>
+      <c r="K180" s="10">
+        <v>41434</v>
+      </c>
+      <c r="L180" s="1">
+        <v>3</v>
+      </c>
+      <c r="M180" s="1">
+        <v>150</v>
+      </c>
+      <c r="N180" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O180" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P180" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q180" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R180" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="S180" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="181" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A181" s="1">
+        <v>8456987</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F181" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G181" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H181" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I181" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J181" s="12">
+        <v>41432</v>
+      </c>
+      <c r="K181" s="10">
+        <v>41434</v>
+      </c>
+      <c r="L181" s="1">
+        <v>3</v>
+      </c>
+      <c r="M181" s="1">
+        <v>150</v>
+      </c>
+      <c r="N181" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O181" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P181" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q181" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R181" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="S181" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="182" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A182" s="1">
+        <v>8456987</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F182" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G182" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H182" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I182" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J182" s="12">
+        <v>41432</v>
+      </c>
+      <c r="K182" s="10">
+        <v>41434</v>
+      </c>
+      <c r="L182" s="1">
+        <v>3</v>
+      </c>
+      <c r="M182" s="1">
+        <v>150</v>
+      </c>
+      <c r="N182" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O182" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P182" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q182" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R182" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="S182" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="183" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A183" s="1">
+        <v>8456987</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F183" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G183" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H183" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I183" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J183" s="12">
+        <v>41432</v>
+      </c>
+      <c r="K183" s="10">
+        <v>41434</v>
+      </c>
+      <c r="L183" s="1">
+        <v>3</v>
+      </c>
+      <c r="M183" s="1">
+        <v>150</v>
+      </c>
+      <c r="N183" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O183" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P183" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q183" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R183" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="S183" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="184" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>8456987</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F184" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G184" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H184" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I184" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J184" s="12">
+        <v>41432</v>
+      </c>
+      <c r="K184" s="10">
+        <v>41434</v>
+      </c>
+      <c r="L184" s="1">
+        <v>3</v>
+      </c>
+      <c r="M184" s="1">
+        <v>150</v>
+      </c>
+      <c r="N184" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O184" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P184" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q184" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R184" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="S184" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>